<commit_message>
commit to get up to speed before re-entering project
</commit_message>
<xml_diff>
--- a/tables/Table1_model_aic_comparison.xlsx
+++ b/tables/Table1_model_aic_comparison.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/forage_fish/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD0997F4-D151-5E49-BB5C-FF3457F5AC85}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F03579-B363-074F-A506-38353143A249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1500" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9320" yWindow="460" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_model_aic_comparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -46,10 +46,83 @@
     <t>PT model (MSY@37%K)</t>
   </si>
   <si>
-    <t>PT model (MSY@45%K)</t>
-  </si>
-  <si>
-    <t>Prey-linked PT model (MSY@45%K)</t>
+    <r>
+      <t xml:space="preserve">PT model (MSY@45%K) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(base model)</t>
+    </r>
+  </si>
+  <si>
+    <t>Question 1: Is productivity symmetric?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PT model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(base model)</t>
+    </r>
+  </si>
+  <si>
+    <t>Prey-linked, random effects PT model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prey-linked, fixed effects PT model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(prey model)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SST-linked, fixed effects PT model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(SST model)</t>
+    </r>
+  </si>
+  <si>
+    <t>SST-linked, random effects PT model</t>
+  </si>
+  <si>
+    <t>Question 2: Does primary prey influence productivity?</t>
+  </si>
+  <si>
+    <t>Question 3: Does primary prey influence productivity as much as SST?</t>
   </si>
 </sst>
 </file>
@@ -59,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,6 +263,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,10 +628,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -906,22 +994,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E7"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E15" sqref="A2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -938,89 +1026,196 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>116</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-1220.7285726385801</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-2209.4571452771602</v>
-      </c>
-      <c r="E3" s="1">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-2018.0157957951601</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-3754.0315915903202</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>87</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-1184.3362555163701</v>
-      </c>
-      <c r="D4" s="1">
-        <v>-2194.6725110327402</v>
-      </c>
-      <c r="E4" s="1">
-        <v>14.7846342444186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-2017.40085022942</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-3752.8017004588501</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.2298911314700973</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>141</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-2015.14826119236</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-3748.29652238473</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5.7350692055892978</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>87</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-1183.61992438783</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-2193.23984877566</v>
-      </c>
-      <c r="E5" s="1">
-        <v>16.217296501498399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>87</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-1182.84340947746</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-2191.68681895492</v>
-      </c>
-      <c r="E6" s="1">
-        <v>17.770326322235199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
       <c r="B7">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1">
-        <v>-1180.7288065226301</v>
+        <v>-2014.4497925426101</v>
       </c>
       <c r="D7" s="1">
-        <v>-2187.4576130452501</v>
+        <v>-3746.8995850852298</v>
       </c>
       <c r="E7" s="1">
-        <v>21.9995322319051</v>
+        <v>7.132006505090402</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>188</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-2076.5339281547299</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-3777.0678563094698</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>143</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-2020.3746073566599</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-3754.7492147133098</v>
+      </c>
+      <c r="E10" s="1">
+        <v>22.318641596157796</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>141</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-2018.0157957951601</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-3754.0315915903202</v>
+      </c>
+      <c r="E11" s="1">
+        <v>23.036264719150999</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>188</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-2101.1576373258599</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-3826.3152746517198</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>143</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-2037.5424142771201</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-3789.0848285542502</v>
+      </c>
+      <c r="E14" s="1">
+        <v>37.230446097471003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>188</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-2076.5339281547299</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-3777.0678563094698</v>
+      </c>
+      <c r="E15" s="1">
+        <v>49.247418342249098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restructured file structure and some other stuff
</commit_message>
<xml_diff>
--- a/tables/Table1_model_aic_comparison.xlsx
+++ b/tables/Table1_model_aic_comparison.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/forage_fish/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F03579-B363-074F-A506-38353143A249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13976240-464C-394A-9B14-5C804CB173B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="460" windowWidth="25040" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16940" yWindow="2220" windowWidth="31820" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_model_aic_comparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Model</t>
   </si>
@@ -65,64 +65,28 @@
     <t>Question 1: Is productivity symmetric?</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">PT model </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(base model)</t>
-    </r>
-  </si>
-  <si>
-    <t>Prey-linked, random effects PT model</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Prey-linked, fixed effects PT model </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(prey model)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SST-linked, fixed effects PT model </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(SST model)</t>
-    </r>
-  </si>
-  <si>
-    <t>SST-linked, random effects PT model</t>
-  </si>
-  <si>
-    <t>Question 2: Does primary prey influence productivity?</t>
-  </si>
-  <si>
     <t>Question 3: Does primary prey influence productivity as much as SST?</t>
+  </si>
+  <si>
+    <t>Question 2: Does prey abundance influence productivity?</t>
+  </si>
+  <si>
+    <t>Primary prey (random effects)</t>
+  </si>
+  <si>
+    <t>Composite prey (fixed effects)</t>
+  </si>
+  <si>
+    <t>Primary prey (fixed effects)</t>
+  </si>
+  <si>
+    <t>Composite prey (random effects)</t>
+  </si>
+  <si>
+    <t>SST (fixed effects)</t>
+  </si>
+  <si>
+    <t>SST (random effects)</t>
   </si>
 </sst>
 </file>
@@ -994,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A2:E15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,8 +969,14 @@
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1036,15 +1006,16 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C4" s="1">
-        <v>-2018.0157957951601</v>
+        <v>-1938.2982727824899</v>
       </c>
       <c r="D4" s="1">
-        <v>-3754.0315915903202</v>
+        <v>-3606.5965455649698</v>
       </c>
       <c r="E4" s="1">
+        <f>0</f>
         <v>0</v>
       </c>
       <c r="F4" s="1"/>
@@ -1054,16 +1025,17 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1">
-        <v>-2017.40085022942</v>
+        <v>-1937.6188498059701</v>
       </c>
       <c r="D5" s="1">
-        <v>-3752.8017004588501</v>
+        <v>-3605.2376996119401</v>
       </c>
       <c r="E5" s="1">
-        <v>1.2298911314700973</v>
+        <f>D5-$L$20</f>
+        <v>-3605.2376996119401</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1072,16 +1044,17 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1">
-        <v>-2015.14826119236</v>
+        <v>-1935.27461961004</v>
       </c>
       <c r="D6" s="1">
-        <v>-3748.29652238473</v>
+        <v>-3600.5492392200699</v>
       </c>
       <c r="E6" s="1">
-        <v>5.7350692055892978</v>
+        <f>D6-$L$20</f>
+        <v>-3600.5492392200699</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1090,36 +1063,38 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C7" s="1">
-        <v>-2014.4497925426101</v>
+        <v>-1934.7503896539499</v>
       </c>
       <c r="D7" s="1">
-        <v>-3746.8995850852298</v>
+        <v>-3599.5007793078898</v>
       </c>
       <c r="E7" s="1">
-        <v>7.132006505090402</v>
+        <f>D7-$L$20</f>
+        <v>-3599.5007793078898</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C9" s="1">
-        <v>-2076.5339281547299</v>
+        <v>-2000.3114680421199</v>
       </c>
       <c r="D9" s="1">
-        <v>-3777.0678563094698</v>
+        <v>-3640.6229360842399</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1128,97 +1103,307 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="C10" s="1">
-        <v>-2020.3746073566599</v>
+        <v>-1997.6983407212599</v>
       </c>
       <c r="D10" s="1">
-        <v>-3754.7492147133098</v>
+        <v>-3635.3966814425298</v>
       </c>
       <c r="E10" s="1">
-        <v>22.318641596157796</v>
+        <f>D10-$L$26</f>
+        <v>-3635.3966814425298</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C11" s="1">
-        <v>-2018.0157957951601</v>
+        <v>-1940.5886472961699</v>
       </c>
       <c r="D11" s="1">
-        <v>-3754.0315915903202</v>
+        <v>-3607.1772945923399</v>
       </c>
       <c r="E11" s="1">
-        <v>23.036264719150999</v>
-      </c>
-      <c r="F11" s="1"/>
+        <f t="shared" ref="E11:E13" si="0">D11-$L$26</f>
+        <v>-3607.1772945923399</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>135</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1938.2982727824899</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-3606.5965455649698</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>-3606.5965455649698</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="C13" s="1">
-        <v>-2101.1576373258599</v>
+        <v>-1940.23242521728</v>
       </c>
       <c r="D13" s="1">
-        <v>-3826.3152746517198</v>
+        <v>-3606.46485043455</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-3606.46485043455</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>143</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-2037.5424142771201</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-3789.0848285542502</v>
-      </c>
-      <c r="E14" s="1">
-        <v>37.230446097471003</v>
+      <c r="A14" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>180</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-2012.0388598215</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-3664.0777196430099</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>180</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-2000.3114680421199</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-3640.6229360842399</v>
+      </c>
+      <c r="E16" s="1">
+        <v>23.454783558768199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>180</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-1997.6983407212599</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-3635.3966814425298</v>
+      </c>
+      <c r="E17" s="1">
+        <v>28.681038200480501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>137</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-1953.5692785495401</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-3633.1385570990701</v>
+      </c>
+      <c r="E18" s="1">
+        <v>30.939162543933399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>188</v>
-      </c>
-      <c r="C15" s="1">
-        <v>-2076.5339281547299</v>
-      </c>
-      <c r="D15" s="1">
-        <v>-3777.0678563094698</v>
-      </c>
-      <c r="E15" s="1">
-        <v>49.247418342249098</v>
-      </c>
+      <c r="B19">
+        <v>137</v>
+      </c>
+      <c r="C19" s="1">
+        <v>-1940.5886472961699</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-3607.1772945923399</v>
+      </c>
+      <c r="E19" s="1">
+        <v>56.900425050672801</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>135</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-1938.2982727824899</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-3606.5965455649698</v>
+      </c>
+      <c r="E20" s="1">
+        <v>57.4811740780356</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-1940.23242521728</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-3606.46485043455</v>
+      </c>
+      <c r="E21" s="1">
+        <v>57.612869208455301</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I22" s="3"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I26" s="3"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I27" s="3"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I28" s="3"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I29" s="3"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I30" s="3"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I33" s="3"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I34" s="3"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I35" s="3"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I36" s="3"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I37" s="3"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I38" s="3"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I39" s="3"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="I26:M30">
+    <sortCondition ref="L26:L30"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
added power analysis and fixed things up before submission
</commit_message>
<xml_diff>
--- a/tables/Table1_model_aic_comparison.xlsx
+++ b/tables/Table1_model_aic_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/forage_fish/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13976240-464C-394A-9B14-5C804CB173B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC3D048-6E7B-7045-AD4A-2CEBEDB9A5EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16940" yWindow="2220" windowWidth="31820" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_model_aic_comparison" sheetId="1" r:id="rId1"/>
@@ -77,16 +77,42 @@
     <t>Composite prey (fixed effects)</t>
   </si>
   <si>
-    <t>Primary prey (fixed effects)</t>
-  </si>
-  <si>
     <t>Composite prey (random effects)</t>
   </si>
   <si>
-    <t>SST (fixed effects)</t>
-  </si>
-  <si>
     <t>SST (random effects)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Primary prey (fixed effects) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(best prey model)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SST (fixed effects) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(best SST model)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -960,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1041,7 @@
         <v>-3606.5965455649698</v>
       </c>
       <c r="E4" s="1">
-        <f>0</f>
+        <f>D4-$D$4</f>
         <v>0</v>
       </c>
       <c r="F4" s="1"/>
@@ -1034,8 +1060,8 @@
         <v>-3605.2376996119401</v>
       </c>
       <c r="E5" s="1">
-        <f>D5-$L$20</f>
-        <v>-3605.2376996119401</v>
+        <f t="shared" ref="E5:E7" si="0">D5-$D$4</f>
+        <v>1.3588459530296859</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1053,8 +1079,8 @@
         <v>-3600.5492392200699</v>
       </c>
       <c r="E6" s="1">
-        <f>D6-$L$20</f>
-        <v>-3600.5492392200699</v>
+        <f t="shared" si="0"/>
+        <v>6.0473063448998801</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -1072,8 +1098,8 @@
         <v>-3599.5007793078898</v>
       </c>
       <c r="E7" s="1">
-        <f>D7-$L$20</f>
-        <v>-3599.5007793078898</v>
+        <f t="shared" si="0"/>
+        <v>7.0957662570799585</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -1085,7 +1111,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>180</v>
@@ -1097,6 +1123,7 @@
         <v>-3640.6229360842399</v>
       </c>
       <c r="E9" s="1">
+        <f>D9-$D$9</f>
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
@@ -1115,8 +1142,8 @@
         <v>-3635.3966814425298</v>
       </c>
       <c r="E10" s="1">
-        <f>D10-$L$26</f>
-        <v>-3635.3966814425298</v>
+        <f t="shared" ref="E10:E13" si="1">D10-$D$9</f>
+        <v>5.2262546417100566</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1134,8 +1161,8 @@
         <v>-3607.1772945923399</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E13" si="0">D11-$L$26</f>
-        <v>-3607.1772945923399</v>
+        <f t="shared" si="1"/>
+        <v>33.445641491900005</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1152,13 +1179,13 @@
         <v>-3606.5965455649698</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>-3606.5965455649698</v>
+        <f t="shared" si="1"/>
+        <v>34.02639051927008</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>137</v>
@@ -1170,8 +1197,8 @@
         <v>-3606.46485043455</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>-3606.46485043455</v>
+        <f t="shared" si="1"/>
+        <v>34.158085649689838</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1181,7 +1208,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>180</v>
@@ -1193,12 +1220,13 @@
         <v>-3664.0777196430099</v>
       </c>
       <c r="E15" s="1">
+        <f>D15-$D$15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>180</v>
@@ -1210,7 +1238,8 @@
         <v>-3640.6229360842399</v>
       </c>
       <c r="E16" s="1">
-        <v>23.454783558768199</v>
+        <f>D16-$D$15</f>
+        <v>23.454783558770032</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1227,12 +1256,13 @@
         <v>-3635.3966814425298</v>
       </c>
       <c r="E17" s="1">
-        <v>28.681038200480501</v>
+        <f>D17-$D$15</f>
+        <v>28.681038200480089</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>137</v>
@@ -1244,7 +1274,8 @@
         <v>-3633.1385570990701</v>
       </c>
       <c r="E18" s="1">
-        <v>30.939162543933399</v>
+        <f>D18-$D$15</f>
+        <v>30.939162543939801</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1261,7 +1292,8 @@
         <v>-3607.1772945923399</v>
       </c>
       <c r="E19" s="1">
-        <v>56.900425050672801</v>
+        <f>D19-$D$15</f>
+        <v>56.900425050670037</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -1279,7 +1311,8 @@
         <v>-3606.5965455649698</v>
       </c>
       <c r="E20" s="1">
-        <v>57.4811740780356</v>
+        <f>D20-$D$15</f>
+        <v>57.481174078040112</v>
       </c>
       <c r="I20" s="3"/>
       <c r="K20" s="1"/>
@@ -1288,7 +1321,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>137</v>
@@ -1300,7 +1333,8 @@
         <v>-3606.46485043455</v>
       </c>
       <c r="E21" s="1">
-        <v>57.612869208455301</v>
+        <f>D21-$D$15</f>
+        <v>57.61286920845987</v>
       </c>
       <c r="I21" s="3"/>
       <c r="K21" s="1"/>

</xml_diff>

<commit_message>
revisions before resubmission - lagged analysis, etc
</commit_message>
<xml_diff>
--- a/tables/Table1_model_aic_comparison.xlsx
+++ b/tables/Table1_model_aic_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/forage_fish/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC3D048-6E7B-7045-AD4A-2CEBEDB9A5EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5006654F-2342-C743-9195-782913120041}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15080" yWindow="3440" windowWidth="36120" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_model_aic_comparison" sheetId="1" r:id="rId1"/>
@@ -25,50 +25,13 @@
     <t>Model</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>Likelihood</t>
-  </si>
-  <si>
     <t>AIC</t>
   </si>
   <si>
-    <t>ΔAIC</t>
-  </si>
-  <si>
-    <t>PT model (MSY@40%K)</t>
-  </si>
-  <si>
-    <t>PT model (MSY@50%K)</t>
-  </si>
-  <si>
-    <t>PT model (MSY@37%K)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">PT model (MSY@45%K) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(base model)</t>
-    </r>
-  </si>
-  <si>
     <t>Question 1: Is productivity symmetric?</t>
   </si>
   <si>
     <t>Question 3: Does primary prey influence productivity as much as SST?</t>
-  </si>
-  <si>
-    <t>Question 2: Does prey abundance influence productivity?</t>
   </si>
   <si>
     <t>Primary prey (random effects)</t>
@@ -114,6 +77,67 @@
       <t>(best SST model)</t>
     </r>
   </si>
+  <si>
+    <t>NLL</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No covariate (MSY@45%K) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(base model)</t>
+    </r>
+  </si>
+  <si>
+    <t>No covariate (MSY@40%K)</t>
+  </si>
+  <si>
+    <t>No covariate (MSY@37%K)</t>
+  </si>
+  <si>
+    <t>No covariate (MSY@50%K)</t>
+  </si>
+  <si>
+    <r>
+      <t>ΔAIC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Question 2: Does prey abundance influence productivity?</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +288,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="33">
@@ -986,59 +1024,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="20" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickTop="1">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>135</v>
       </c>
       <c r="C4" s="1">
-        <v>-1938.2982727824899</v>
+        <v>-1938.2982727824699</v>
       </c>
       <c r="D4" s="1">
-        <v>-3606.5965455649698</v>
+        <v>-3606.5965455649498</v>
       </c>
       <c r="E4" s="1">
         <f>D4-$D$4</f>
@@ -1046,18 +1084,18 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>135</v>
       </c>
       <c r="C5" s="1">
-        <v>-1937.6188498059701</v>
+        <v>-1937.6188498059601</v>
       </c>
       <c r="D5" s="1">
-        <v>-3605.2376996119401</v>
+        <v>-3605.2376996119201</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E7" si="0">D5-$D$4</f>
@@ -1065,37 +1103,37 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>135</v>
       </c>
       <c r="C6" s="1">
-        <v>-1935.27461961004</v>
+        <v>-1935.27461961002</v>
       </c>
       <c r="D6" s="1">
-        <v>-3600.5492392200699</v>
+        <v>-3600.5492392200399</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>6.0473063448998801</v>
+        <v>6.0473063449098845</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>135</v>
       </c>
       <c r="C7" s="1">
-        <v>-1934.7503896539499</v>
+        <v>-1934.7503896539299</v>
       </c>
       <c r="D7" s="1">
-        <v>-3599.5007793078898</v>
+        <v>-3599.5007793078698</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
@@ -1103,24 +1141,24 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="19">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>180</v>
       </c>
       <c r="C9" s="1">
-        <v>-2000.3114680421199</v>
+        <v>-2000.3114680420699</v>
       </c>
       <c r="D9" s="1">
-        <v>-3640.6229360842399</v>
+        <v>-3640.6229360841398</v>
       </c>
       <c r="E9" s="1">
         <f>D9-$D$9</f>
@@ -1128,307 +1166,307 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>180</v>
       </c>
       <c r="C10" s="1">
-        <v>-1997.6983407212599</v>
+        <v>-1997.6983407212199</v>
       </c>
       <c r="D10" s="1">
-        <v>-3635.3966814425298</v>
+        <v>-3635.3966814424398</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:E13" si="1">D10-$D$9</f>
-        <v>5.2262546417100566</v>
+        <v>5.2262546417000522</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>137</v>
       </c>
       <c r="C11" s="1">
-        <v>-1940.5886472961699</v>
+        <v>-1940.5886472961599</v>
       </c>
       <c r="D11" s="1">
-        <v>-3607.1772945923399</v>
+        <v>-3607.1772945923199</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>33.445641491900005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33.44564149181997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>135</v>
       </c>
       <c r="C12" s="1">
-        <v>-1938.2982727824899</v>
+        <v>-1938.2982727824699</v>
       </c>
       <c r="D12" s="1">
-        <v>-3606.5965455649698</v>
+        <v>-3606.5965455649498</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>34.02639051927008</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34.026390519190045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>137</v>
       </c>
       <c r="C13" s="1">
-        <v>-1940.23242521728</v>
+        <v>-1940.23242521726</v>
       </c>
       <c r="D13" s="1">
-        <v>-3606.46485043455</v>
+        <v>-3606.46485043451</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>34.158085649689838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34.158085649629811</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>180</v>
       </c>
       <c r="C15" s="1">
-        <v>-2012.0388598215</v>
+        <v>-2006.4501837577</v>
       </c>
       <c r="D15" s="1">
-        <v>-3664.0777196430099</v>
+        <v>-3652.9003675153999</v>
       </c>
       <c r="E15" s="1">
-        <f>D15-$D$15</f>
+        <f t="shared" ref="E15:E21" si="2">D15-$D$15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>180</v>
       </c>
       <c r="C16" s="1">
-        <v>-2000.3114680421199</v>
+        <v>-2000.3114680420699</v>
       </c>
       <c r="D16" s="1">
-        <v>-3640.6229360842399</v>
+        <v>-3640.6229360841398</v>
       </c>
       <c r="E16" s="1">
-        <f>D16-$D$15</f>
-        <v>23.454783558770032</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>12.277431431260084</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>180</v>
       </c>
       <c r="C17" s="1">
-        <v>-1997.6983407212599</v>
+        <v>-1997.6983407212199</v>
       </c>
       <c r="D17" s="1">
-        <v>-3635.3966814425298</v>
+        <v>-3635.3966814424398</v>
       </c>
       <c r="E17" s="1">
-        <f>D17-$D$15</f>
-        <v>28.681038200480089</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>17.503686072960136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>137</v>
       </c>
       <c r="C18" s="1">
-        <v>-1953.5692785495401</v>
+        <v>-1947.33859556831</v>
       </c>
       <c r="D18" s="1">
-        <v>-3633.1385570990701</v>
+        <v>-3620.67719113662</v>
       </c>
       <c r="E18" s="1">
-        <f>D18-$D$15</f>
-        <v>30.939162543939801</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>32.223176378779954</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>137</v>
       </c>
       <c r="C19" s="1">
-        <v>-1940.5886472961699</v>
+        <v>-1940.5886472961599</v>
       </c>
       <c r="D19" s="1">
-        <v>-3607.1772945923399</v>
+        <v>-3607.1772945923199</v>
       </c>
       <c r="E19" s="1">
-        <f>D19-$D$15</f>
-        <v>56.900425050670037</v>
+        <f t="shared" si="2"/>
+        <v>45.723072923080053</v>
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>135</v>
       </c>
       <c r="C20" s="1">
-        <v>-1938.2982727824899</v>
+        <v>-1938.2982727824699</v>
       </c>
       <c r="D20" s="1">
-        <v>-3606.5965455649698</v>
+        <v>-3606.5965455649498</v>
       </c>
       <c r="E20" s="1">
-        <f>D20-$D$15</f>
-        <v>57.481174078040112</v>
+        <f t="shared" si="2"/>
+        <v>46.303821950450128</v>
       </c>
       <c r="I20" s="3"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>137</v>
       </c>
       <c r="C21" s="1">
-        <v>-1940.23242521728</v>
+        <v>-1940.23242521726</v>
       </c>
       <c r="D21" s="1">
-        <v>-3606.46485043455</v>
+        <v>-3606.46485043451</v>
       </c>
       <c r="E21" s="1">
-        <f>D21-$D$15</f>
-        <v>57.61286920845987</v>
+        <f t="shared" si="2"/>
+        <v>46.435517080889895</v>
       </c>
       <c r="I21" s="3"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="I22" s="3"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="I23" s="3"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="I26" s="3"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="I27" s="3"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="I28" s="3"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="I29" s="3"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="I30" s="3"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="9:13">
       <c r="I33" s="3"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="9:13">
       <c r="I34" s="3"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="9:13">
       <c r="I35" s="3"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="9:13">
       <c r="I36" s="3"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="9:13">
       <c r="I37" s="3"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="9:13">
       <c r="I38" s="3"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="9:13">
       <c r="I39" s="3"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>

</xml_diff>